<commit_message>
Fix backend issues and enhance face recognition
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1640,6 +1640,23 @@
         </is>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Kartikey Gupta</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>19:00:22</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Production-ready face attendance system
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1657,6 +1657,40 @@
         </is>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Kartikey Gupta</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>20:32:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Kartikey Gupta</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>20:42:40</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>